<commit_message>
Feat: Merge functionality of manipulating letters
Co-authored-by: moris mwai <moris.wachira@griffinglobaltech.com>
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\Onboarding_Email_Handler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AF6DF-47E5-447D-A223-E49B2B5231D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="-13665" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
   </si>
   <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
@@ -159,7 +156,34 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>HROnboarding</t>
+  </si>
+  <si>
+    <t>ExcelPath</t>
+  </si>
+  <si>
+    <t>EmailCredentials</t>
+  </si>
+  <si>
+    <t>EmailSubject</t>
+  </si>
+  <si>
+    <t>Data\Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>EmailBody</t>
+  </si>
+  <si>
+    <t>Hello, 
+An exception occurred during the automation process.  Please find the details below:
+Exception Source: @Source
+Exception Message: @Message
+A screenshot of the error has been attached for reference. Please see the attachment for more details.
+Thank you and have a good day,
+Robot :)</t>
+  </si>
+  <si>
+    <t>Automation Error!</t>
   </si>
 </sst>
 </file>
@@ -212,10 +236,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,7 +562,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,34 +609,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1619,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1673,18 +1697,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1693,118 +1717,132 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,7 +2820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2800,7 +2840,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2828,8 +2868,22 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
finalized on #2 and#7
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\Onboarding_Email_Handler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AF6DF-47E5-447D-A223-E49B2B5231D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C299EE-9128-45A1-8301-22B12F854F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="-13665" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -185,12 +185,58 @@
   <si>
     <t>Automation Error!</t>
   </si>
+  <si>
+    <t>SE_Email_Subject</t>
+  </si>
+  <si>
+    <t>Hired_Email_Body</t>
+  </si>
+  <si>
+    <t>Rejected_Email_Subject</t>
+  </si>
+  <si>
+    <t>From_Email</t>
+  </si>
+  <si>
+    <t>Hired_Email_Subject</t>
+  </si>
+  <si>
+    <t>Test Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dear Candidate
+Thank you for your interest in The Jitu. You have been accepted to proceed to the next stage of the recruitment. We would like to extend our congratulations for making it to this stage..
+Find the attachment for more details.
+Kind Regards,
+Talent Team, TheJitu.
+</t>
+  </si>
+  <si>
+    <t>Dear Candidate
+We received an overwhelming number of responses, which makes us feel both humble and proud that so many talented individuals (you included) want to join our team. We know how much effort goes into each application and we appreciate the time taken to contact us. This volume of responses makes for an extremely competitive selection process. Although your profile is impressive, we regret to inform you that we have decided to pursue other candidates for the position at this time.
+However, we are always keen on hearing from talented people and therefore, we strongly encourage you to continue applying for other vacancies advertised on our career website in an area that matches your skillset and experience. Also remember to keep your profile up to date so you can be the first to hear about new job openings.
+Once again, thank you so much for investing your time to make this application. Let’s keep in touch and hopefully we’ll speak again in the near future.
+Kind Regards,
+TheJitu Talent Team.</t>
+  </si>
+  <si>
+    <t>emilytiampati@outlook.com</t>
+  </si>
+  <si>
+    <t>Congratulations You've Been Accepted!</t>
+  </si>
+  <si>
+    <t>Automation error!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello, </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,6 +260,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,10 +284,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -245,8 +298,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -263,9 +318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -303,7 +358,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -409,7 +464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -551,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,12 +620,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -618,7 +673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -628,7 +683,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1644,15 +1699,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1689,7 +1744,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1700,7 +1755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1814,7 +1869,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1843,13 +1898,62 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2812,6 +2916,9 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" xr:uid="{D7CA06A5-626A-4828-9624-A0A883662C40}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2824,12 +2931,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Update the Candidate Summary List #3
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\Onboarding_Email_Handler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AF6DF-47E5-447D-A223-E49B2B5231D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37F2674-FB80-4110-A353-3DDCA39204E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="-13665" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Automation Error!</t>
+  </si>
+  <si>
+    <t>inputSheet</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
@@ -263,9 +269,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -303,7 +309,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -409,7 +415,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -551,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,15 +568,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -618,7 +624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -628,7 +634,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1644,15 +1650,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1689,7 +1695,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1700,7 +1706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1814,7 +1820,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1843,7 +1849,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2824,12 +2837,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
updated the config file with inputsheet constant
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37F2674-FB80-4110-A353-3DDCA39204E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF54A49D-9EEA-4EC9-A079-B79C4A73AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,7 +1650,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1849,14 +1849,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1864,7 +1857,14 @@
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added .local iin gitignore
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF54A49D-9EEA-4EC9-A079-B79C4A73AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA969E54-4327-45A9-908A-168921940B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1650,7 +1650,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1857,32 +1857,32 @@
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updating the candidate summary list file #3
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C299EE-9128-45A1-8301-22B12F854F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D88A824-44AC-4902-AC76-9C3E780F2AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t xml:space="preserve">Hello, </t>
+  </si>
+  <si>
+    <t>inputSheet</t>
+  </si>
+  <si>
+    <t>sheet1</t>
   </si>
 </sst>
 </file>
@@ -1698,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1955,7 +1961,14 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
cleaned up the workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D88A824-44AC-4902-AC76-9C3E780F2AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E9D57-E6D3-405F-910E-691A463DF33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -229,13 +229,16 @@
     <t>Automation error!</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello, </t>
-  </si>
-  <si>
     <t>inputSheet</t>
   </si>
   <si>
     <t>sheet1</t>
+  </si>
+  <si>
+    <t>File_Not_Found_Email_Body</t>
+  </si>
+  <si>
+    <t>Hello, The Candidate Summary List excel file was not found.</t>
   </si>
 </sst>
 </file>
@@ -324,9 +327,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +473,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1705,7 +1708,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1954,19 +1957,19 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
         <v>63</v>
-      </c>
-      <c r="B30" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Feat : Added Deleted files & Update Candidate Excel xaml workflows
* updating the candidate summary list file #3

* finalized on implementing updating candidates summary list

* cleaned up the workflow

* added the workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C299EE-9128-45A1-8301-22B12F854F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E9D57-E6D3-405F-910E-691A463DF33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -229,7 +229,16 @@
     <t>Automation error!</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello, </t>
+    <t>inputSheet</t>
+  </si>
+  <si>
+    <t>sheet1</t>
+  </si>
+  <si>
+    <t>File_Not_Found_Email_Body</t>
+  </si>
+  <si>
+    <t>Hello, The Candidate Summary List excel file was not found.</t>
   </si>
 </sst>
 </file>
@@ -318,9 +327,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +473,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1698,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1948,14 +1957,21 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
changed the queue and folder name in the config file for integration purposes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E9D57-E6D3-405F-910E-691A463DF33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E30BB1-CC35-41A6-9B5C-632DDC84C7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>HROnboarding</t>
   </si>
   <si>
     <t>ExcelPath</t>
@@ -239,6 +236,12 @@
   </si>
   <si>
     <t>Hello, The Candidate Summary List excel file was not found.</t>
+  </si>
+  <si>
+    <t>CandidatesQueue</t>
+  </si>
+  <si>
+    <t>OnboardingEmailCoordinator</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -676,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -686,7 +689,9 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1708,7 +1713,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1781,7 +1786,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1893,83 +1898,83 @@
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
         <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2993,18 +2998,18 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Modifications based on dispatcher
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E9D57-E6D3-405F-910E-691A463DF33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4CF8D9-A085-456D-8ACE-D7BAA5432381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-195" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -156,19 +156,10 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>HROnboarding</t>
-  </si>
-  <si>
-    <t>ExcelPath</t>
-  </si>
-  <si>
     <t>EmailCredentials</t>
   </si>
   <si>
     <t>EmailSubject</t>
-  </si>
-  <si>
-    <t>Data\Exceptions_Screenshots</t>
   </si>
   <si>
     <t>EmailBody</t>
@@ -226,9 +217,6 @@
     <t>Congratulations You've Been Accepted!</t>
   </si>
   <si>
-    <t>Automation error!</t>
-  </si>
-  <si>
     <t>inputSheet</t>
   </si>
   <si>
@@ -239,6 +227,18 @@
   </si>
   <si>
     <t>Hello, The Candidate Summary List excel file was not found.</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>OnboardingEmailCoordinator</t>
+  </si>
+  <si>
+    <t>CandidatesQueue</t>
+  </si>
+  <si>
+    <t>str_ExcelCandidatePath</t>
   </si>
 </sst>
 </file>
@@ -626,15 +626,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -676,23 +676,25 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1705,18 +1707,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1753,7 +1755,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1764,7 +1766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1878,7 +1880,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1893,85 +1895,78 @@
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -2929,7 +2924,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -2943,16 +2937,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2993,18 +2987,18 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
+        <v>65</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
fix: Resolve folder non-existence issue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0099E77B-B9F3-4851-A265-8B6A39261C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708A4F0F-57F0-4043-9B76-C2E527D2CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3096" yWindow="2304" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Rejected_Email_Subject</t>
   </si>
   <si>
-    <t>From_Email</t>
-  </si>
-  <si>
     <t>Hired_Email_Subject</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
     <t>Hello, The Candidate Summary List excel file was not found.</t>
   </si>
   <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
     <t>CandidatesQueue</t>
   </si>
   <si>
@@ -233,9 +233,6 @@
   </si>
   <si>
     <t>str_ExcelCandidatePath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
   </si>
 </sst>
 </file>
@@ -626,12 +623,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -679,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -691,7 +688,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1706,16 +1703,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,7 +1749,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1763,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1780,7 +1777,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1877,7 +1874,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1904,7 +1901,7 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -1912,7 +1909,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -1920,7 +1917,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -1928,10 +1925,10 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -1939,24 +1936,24 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2925,18 +2922,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2976,7 +2974,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B2" t="s">
@@ -2991,14 +2989,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3998,5 +3989,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Resolve folder non-existence issue (#10)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0099E77B-B9F3-4851-A265-8B6A39261C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708A4F0F-57F0-4043-9B76-C2E527D2CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16350" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3096" yWindow="2304" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Rejected_Email_Subject</t>
   </si>
   <si>
-    <t>From_Email</t>
-  </si>
-  <si>
     <t>Hired_Email_Subject</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
     <t>Hello, The Candidate Summary List excel file was not found.</t>
   </si>
   <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
     <t>CandidatesQueue</t>
   </si>
   <si>
@@ -233,9 +233,6 @@
   </si>
   <si>
     <t>str_ExcelCandidatePath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
   </si>
 </sst>
 </file>
@@ -626,12 +623,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -679,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -691,7 +688,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1706,16 +1703,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,7 +1749,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1763,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1780,7 +1777,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1877,7 +1874,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1904,7 +1901,7 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -1912,7 +1909,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -1920,7 +1917,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -1928,10 +1925,10 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -1939,24 +1936,24 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2925,18 +2922,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2976,7 +2974,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B2" t="s">
@@ -2991,14 +2989,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3998,5 +3989,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
worked on updating the db with candidates and automation details
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingEmailHandler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708A4F0F-57F0-4043-9B76-C2E527D2CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD763EB-241C-4A81-A986-01D7E1D43DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3096" yWindow="2304" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -233,6 +233,13 @@
   </si>
   <si>
     <t>str_ExcelCandidatePath</t>
+  </si>
+  <si>
+    <t>update_db</t>
+  </si>
+  <si>
+    <t>INSERT INTO [dbo].[Reports] ([ID], [FullName], [Email], [JobStatus], [AcceptanceDeadline], [StartDate], [Address], [BotName], [TimeStamp])
+VALUES (@ID, @FullName, @Email, @JobStatus, @AcceptanceDeadline, @StartDate, @Address, @BotName, GETDATE());</t>
   </si>
 </sst>
 </file>
@@ -623,12 +630,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -676,7 +683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -688,7 +695,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1703,16 +1710,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1749,7 +1756,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1760,7 +1767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1874,7 +1881,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1956,7 +1963,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -2925,16 +2939,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Performer update updating candidate data in db (#12)
* added database nuget package and database activities to connect to db

* worked on updating the db with candidates and automation details

* updated the updating data to db file to use dynamic values in the query
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingEmailHandler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708A4F0F-57F0-4043-9B76-C2E527D2CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD763EB-241C-4A81-A986-01D7E1D43DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3096" yWindow="2304" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -233,6 +233,13 @@
   </si>
   <si>
     <t>str_ExcelCandidatePath</t>
+  </si>
+  <si>
+    <t>update_db</t>
+  </si>
+  <si>
+    <t>INSERT INTO [dbo].[Reports] ([ID], [FullName], [Email], [JobStatus], [AcceptanceDeadline], [StartDate], [Address], [BotName], [TimeStamp])
+VALUES (@ID, @FullName, @Email, @JobStatus, @AcceptanceDeadline, @StartDate, @Address, @BotName, GETDATE());</t>
   </si>
 </sst>
 </file>
@@ -623,12 +630,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -676,7 +683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -688,7 +695,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1703,16 +1710,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1749,7 +1756,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1760,7 +1767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1874,7 +1881,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1956,7 +1963,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -2925,16 +2939,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
completed the #11 Performer Update : Change from updating Candidate Summary Excel file to updating the candidate data in Db
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD763EB-241C-4A81-A986-01D7E1D43DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC3529-56C5-4B6C-B16D-9F8D9771A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -240,6 +240,28 @@
   <si>
     <t>INSERT INTO [dbo].[Reports] ([ID], [FullName], [Email], [JobStatus], [AcceptanceDeadline], [StartDate], [Address], [BotName], [TimeStamp])
 VALUES (@ID, @FullName, @Email, @JobStatus, @AcceptanceDeadline, @StartDate, @Address, @BotName, GETDATE());</t>
+  </si>
+  <si>
+    <t>UpdateExceptionTable_Query</t>
+  </si>
+  <si>
+    <t>INSERT INTO [CandidateSummaryDB].[dbo].[Exceptions] ([ExceptionID], [BotName], [ExceptionMessage], [ExceptionType], [Source], [StartTime], [EndTime])
+VALUES (@ExceptionID, @BotName, @ExceptionMessage, @ExceptionType, @Source, @StartTime, GETDATE() AT TIME ZONE 'UTC' AT TIME ZONE 'E. Africa Standard Time');</t>
+  </si>
+  <si>
+    <t>SET IDENTITY_INSERT [CandidateSummaryDB].[dbo].[Reports] ON;
+UPDATE [CandidateSummaryDB].[dbo].[Reports]
+SET 
+	[TimeStamp] = GETDATE() AT TIME ZONE 'UTC' AT TIME ZONE 'E. Africa Standard Time',
+    [StartTime] = @StartTime,
+    [EndTime] = GETDATE() AT TIME ZONE 'UTC' AT TIME ZONE 'E. Africa Standard Time',
+    [LastUpdatedBot] = @LastUpdatedBot,
+    [AutomationStatus] = @AutomationStatus
+WHERE
+    [ID] = @ID;</t>
+  </si>
+  <si>
+    <t>UpdateCandidatesTable_Query</t>
   </si>
 </sst>
 </file>
@@ -1710,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1971,23 +1993,37 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2940,7 +2976,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
completed the #11 Performer Update : Change from updating Candidate Summary Excel file to updating the candidate data in Db (#14)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD763EB-241C-4A81-A986-01D7E1D43DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC3529-56C5-4B6C-B16D-9F8D9771A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -240,6 +240,28 @@
   <si>
     <t>INSERT INTO [dbo].[Reports] ([ID], [FullName], [Email], [JobStatus], [AcceptanceDeadline], [StartDate], [Address], [BotName], [TimeStamp])
 VALUES (@ID, @FullName, @Email, @JobStatus, @AcceptanceDeadline, @StartDate, @Address, @BotName, GETDATE());</t>
+  </si>
+  <si>
+    <t>UpdateExceptionTable_Query</t>
+  </si>
+  <si>
+    <t>INSERT INTO [CandidateSummaryDB].[dbo].[Exceptions] ([ExceptionID], [BotName], [ExceptionMessage], [ExceptionType], [Source], [StartTime], [EndTime])
+VALUES (@ExceptionID, @BotName, @ExceptionMessage, @ExceptionType, @Source, @StartTime, GETDATE() AT TIME ZONE 'UTC' AT TIME ZONE 'E. Africa Standard Time');</t>
+  </si>
+  <si>
+    <t>SET IDENTITY_INSERT [CandidateSummaryDB].[dbo].[Reports] ON;
+UPDATE [CandidateSummaryDB].[dbo].[Reports]
+SET 
+	[TimeStamp] = GETDATE() AT TIME ZONE 'UTC' AT TIME ZONE 'E. Africa Standard Time',
+    [StartTime] = @StartTime,
+    [EndTime] = GETDATE() AT TIME ZONE 'UTC' AT TIME ZONE 'E. Africa Standard Time',
+    [LastUpdatedBot] = @LastUpdatedBot,
+    [AutomationStatus] = @AutomationStatus
+WHERE
+    [ID] = @ID;</t>
+  </si>
+  <si>
+    <t>UpdateCandidatesTable_Query</t>
   </si>
 </sst>
 </file>
@@ -1710,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1971,23 +1993,37 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2940,7 +2976,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Initial setup: REFramework (C#), Config, README, .gitignore, Excel template
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmillyTiampati\Documents\UiPath\OnboardingEmailHandler\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/OnboardingEmailHandler/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC3529-56C5-4B6C-B16D-9F8D9771A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7EEC3529-56C5-4B6C-B16D-9F8D9771A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED93A89-C63E-49B0-907E-7CD353B70CF7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -279,6 +279,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -297,6 +298,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -652,12 +654,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -705,7 +707,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -717,7 +719,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1732,16 +1734,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1778,7 +1780,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1789,7 +1791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1903,7 +1905,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1918,10 +1920,10 @@
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1961,10 +1963,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2979,12 +2981,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>